<commit_message>
Fixed Subsegment Forecast Problem
Added localOnly=true parameter to named ranges
</commit_message>
<xml_diff>
--- a/Prototype/PHPSCRIPTS/SamanAndrey/Jason/ForecastResult2017.xlsx
+++ b/Prototype/PHPSCRIPTS/SamanAndrey/Jason/ForecastResult2017.xlsx
@@ -22,10 +22,58 @@
     <sheet name="GRPO" sheetId="13" r:id="rId16"/>
   </sheets>
   <definedNames>
-    <definedName name="timeline">'GRPO'!$A$2:$A$4</definedName>
-    <definedName name="rns">'GRPO'!$B$2:$B$4</definedName>
-    <definedName name="arr">'GRPO'!$C$2:$C$4</definedName>
-    <definedName name="rev">'GRPO'!$D$2:$D$4</definedName>
+    <definedName name="timeline" localSheetId="0">'RCK'!$A$2:$A$4</definedName>
+    <definedName name="rns" localSheetId="0">'RCK'!$B$2:$B$4</definedName>
+    <definedName name="arr" localSheetId="0">'RCK'!$C$2:$C$4</definedName>
+    <definedName name="rev" localSheetId="0">'RCK'!$D$2:$D$4</definedName>
+    <definedName name="timeline" localSheetId="1">'CORP'!$A$2:$A$4</definedName>
+    <definedName name="rns" localSheetId="1">'CORP'!$B$2:$B$4</definedName>
+    <definedName name="arr" localSheetId="1">'CORP'!$C$2:$C$4</definedName>
+    <definedName name="rev" localSheetId="1">'CORP'!$D$2:$D$4</definedName>
+    <definedName name="timeline" localSheetId="2">'CORPO'!$A$2:$A$4</definedName>
+    <definedName name="rns" localSheetId="2">'CORPO'!$B$2:$B$4</definedName>
+    <definedName name="arr" localSheetId="2">'CORPO'!$C$2:$C$4</definedName>
+    <definedName name="rev" localSheetId="2">'CORPO'!$D$2:$D$4</definedName>
+    <definedName name="timeline" localSheetId="3">'PKG-PRM'!$A$2:$A$4</definedName>
+    <definedName name="rns" localSheetId="3">'PKG-PRM'!$B$2:$B$4</definedName>
+    <definedName name="arr" localSheetId="3">'PKG-PRM'!$C$2:$C$4</definedName>
+    <definedName name="rev" localSheetId="3">'PKG-PRM'!$D$2:$D$4</definedName>
+    <definedName name="timeline" localSheetId="4">'WSOL'!$A$2:$A$4</definedName>
+    <definedName name="rns" localSheetId="4">'WSOL'!$B$2:$B$4</definedName>
+    <definedName name="arr" localSheetId="4">'WSOL'!$C$2:$C$4</definedName>
+    <definedName name="rev" localSheetId="4">'WSOL'!$D$2:$D$4</definedName>
+    <definedName name="timeline" localSheetId="5">'WSOF'!$A$2:$A$4</definedName>
+    <definedName name="rns" localSheetId="5">'WSOF'!$B$2:$B$4</definedName>
+    <definedName name="arr" localSheetId="5">'WSOF'!$C$2:$C$4</definedName>
+    <definedName name="rev" localSheetId="5">'WSOF'!$D$2:$D$4</definedName>
+    <definedName name="timeline" localSheetId="6">'INDO'!$A$2:$A$4</definedName>
+    <definedName name="rns" localSheetId="6">'INDO'!$B$2:$B$4</definedName>
+    <definedName name="arr" localSheetId="6">'INDO'!$C$2:$C$4</definedName>
+    <definedName name="rev" localSheetId="6">'INDO'!$D$2:$D$4</definedName>
+    <definedName name="timeline" localSheetId="7">'INDR'!$A$2:$A$4</definedName>
+    <definedName name="rns" localSheetId="7">'INDR'!$B$2:$B$4</definedName>
+    <definedName name="arr" localSheetId="7">'INDR'!$C$2:$C$4</definedName>
+    <definedName name="rev" localSheetId="7">'INDR'!$D$2:$D$4</definedName>
+    <definedName name="timeline" localSheetId="8">'CORPM'!$A$2:$A$4</definedName>
+    <definedName name="rns" localSheetId="8">'CORPM'!$B$2:$B$4</definedName>
+    <definedName name="arr" localSheetId="8">'CORPM'!$C$2:$C$4</definedName>
+    <definedName name="rev" localSheetId="8">'CORPM'!$D$2:$D$4</definedName>
+    <definedName name="timeline" localSheetId="9">'CON-ASSOC'!$A$2:$A$4</definedName>
+    <definedName name="rns" localSheetId="9">'CON-ASSOC'!$B$2:$B$4</definedName>
+    <definedName name="arr" localSheetId="9">'CON-ASSOC'!$C$2:$C$4</definedName>
+    <definedName name="rev" localSheetId="9">'CON-ASSOC'!$D$2:$D$4</definedName>
+    <definedName name="timeline" localSheetId="10">'GOV-NGO'!$A$2:$A$4</definedName>
+    <definedName name="rns" localSheetId="10">'GOV-NGO'!$B$2:$B$4</definedName>
+    <definedName name="arr" localSheetId="10">'GOV-NGO'!$C$2:$C$4</definedName>
+    <definedName name="rev" localSheetId="10">'GOV-NGO'!$D$2:$D$4</definedName>
+    <definedName name="timeline" localSheetId="11">'GRPT'!$A$2:$A$4</definedName>
+    <definedName name="rns" localSheetId="11">'GRPT'!$B$2:$B$4</definedName>
+    <definedName name="arr" localSheetId="11">'GRPT'!$C$2:$C$4</definedName>
+    <definedName name="rev" localSheetId="11">'GRPT'!$D$2:$D$4</definedName>
+    <definedName name="timeline" localSheetId="12">'GRPO'!$A$2:$A$4</definedName>
+    <definedName name="rns" localSheetId="12">'GRPO'!$B$2:$B$4</definedName>
+    <definedName name="arr" localSheetId="12">'GRPO'!$C$2:$C$4</definedName>
+    <definedName name="rev" localSheetId="12">'GRPO'!$D$2:$D$4</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>

</xml_diff>